<commit_message>
MainBoardSCH: Change UTS, BUTTONS and IMU_INT pins, swap BUTTON-ON and BUTTON-OFF at JP21, swap SCL and SDA at X3, swap GPIO-1 and GPIO-7 between JP28 and JP30 MainBoardBRD: routing (buses, buttons and LEDs done)
</commit_message>
<xml_diff>
--- a/ele/MainBoard/pinout.xlsx
+++ b/ele/MainBoard/pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\RB3204-RBCX\ele\MainBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C490D586-C66F-443E-A96F-48D704C62010}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B2D46D-5FAD-42D6-8A1F-06D491B456FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{08978B24-E42F-429B-A3F9-EF8F7AA6C2ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{08978B24-E42F-429B-A3F9-EF8F7AA6C2ED}"/>
   </bookViews>
   <sheets>
     <sheet name="koprocesor" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="491">
   <si>
     <t>GPIO</t>
   </si>
@@ -1000,9 +1000,6 @@
   </si>
   <si>
     <t>USART1_RX</t>
-  </si>
-  <si>
-    <t>PE7/TIM1_ETR</t>
   </si>
   <si>
     <t>PE15/TIM1_BKIN</t>
@@ -1736,7 +1733,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -2233,11 +2230,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2457,6 +2478,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2481,63 +2554,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2559,7 +2581,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -2879,9 +2905,9 @@
   </sheetPr>
   <dimension ref="A1:AV114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF103" sqref="AF103"/>
+      <selection pane="bottomLeft" activeCell="AJ96" sqref="AJ96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2910,90 +2936,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="127" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="142" t="s">
+      <c r="B1" s="119" t="s">
         <v>259</v>
       </c>
       <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="138" t="s">
+      <c r="D1" s="129" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="140"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="138" t="s">
+      <c r="E1" s="131"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="129" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="138" t="s">
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="129" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="140"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="138" t="s">
+      <c r="L1" s="131"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="129" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="139"/>
-      <c r="P1" s="125" t="s">
+      <c r="O1" s="130"/>
+      <c r="P1" s="123" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="125" t="s">
+      <c r="Q1" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="R1" s="127" t="s">
+      <c r="R1" s="125" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="128"/>
-      <c r="T1" s="127" t="s">
+      <c r="S1" s="126"/>
+      <c r="T1" s="125" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="128"/>
-      <c r="V1" s="138" t="s">
+      <c r="U1" s="126"/>
+      <c r="V1" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="W1" s="140"/>
-      <c r="X1" s="139"/>
-      <c r="Y1" s="125" t="s">
+      <c r="W1" s="131"/>
+      <c r="X1" s="130"/>
+      <c r="Y1" s="123" t="s">
+        <v>306</v>
+      </c>
+      <c r="Z1" s="123" t="s">
         <v>307</v>
       </c>
-      <c r="Z1" s="125" t="s">
-        <v>308</v>
-      </c>
-      <c r="AA1" s="127" t="s">
+      <c r="AA1" s="125" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="135"/>
-      <c r="AC1" s="128"/>
-      <c r="AD1" s="127" t="s">
+      <c r="AB1" s="134"/>
+      <c r="AC1" s="126"/>
+      <c r="AD1" s="125" t="s">
         <v>124</v>
       </c>
-      <c r="AE1" s="128"/>
+      <c r="AE1" s="126"/>
       <c r="AF1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="AG1" s="129" t="s">
+      <c r="AG1" s="135" t="s">
         <v>125</v>
       </c>
-      <c r="AH1" s="130"/>
-      <c r="AI1" s="133" t="s">
+      <c r="AH1" s="136"/>
+      <c r="AI1" s="132" t="s">
         <v>126</v>
       </c>
-      <c r="AJ1" s="129" t="s">
+      <c r="AJ1" s="135" t="s">
         <v>127</v>
       </c>
-      <c r="AK1" s="130"/>
-      <c r="AL1" s="125" t="s">
+      <c r="AK1" s="136"/>
+      <c r="AL1" s="123" t="s">
         <v>129</v>
       </c>
-      <c r="AM1" s="131" t="s">
+      <c r="AM1" s="145" t="s">
         <v>130</v>
       </c>
-      <c r="AN1" s="133" t="s">
+      <c r="AN1" s="132" t="s">
         <v>151</v>
       </c>
       <c r="AO1" s="8" t="s">
@@ -3008,22 +3034,22 @@
       <c r="AR1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="AS1" s="117" t="s">
+      <c r="AS1" s="137" t="s">
         <v>141</v>
       </c>
-      <c r="AT1" s="119" t="s">
+      <c r="AT1" s="139" t="s">
         <v>182</v>
       </c>
-      <c r="AU1" s="121" t="s">
+      <c r="AU1" s="141" t="s">
         <v>183</v>
       </c>
-      <c r="AV1" s="123" t="s">
+      <c r="AV1" s="143" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="137"/>
-      <c r="B2" s="143"/>
+      <c r="A2" s="128"/>
+      <c r="B2" s="120"/>
       <c r="C2" s="37" t="s">
         <v>96</v>
       </c>
@@ -3063,8 +3089,8 @@
       <c r="O2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="126"/>
+      <c r="P2" s="124"/>
+      <c r="Q2" s="124"/>
       <c r="R2" s="9" t="s">
         <v>105</v>
       </c>
@@ -3086,8 +3112,8 @@
       <c r="X2" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="126"/>
+      <c r="Y2" s="124"/>
+      <c r="Z2" s="124"/>
       <c r="AA2" s="9" t="s">
         <v>101</v>
       </c>
@@ -3110,24 +3136,24 @@
       <c r="AH2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AI2" s="134"/>
+      <c r="AI2" s="133"/>
       <c r="AJ2" s="9" t="s">
         <v>105</v>
       </c>
       <c r="AK2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AL2" s="126"/>
-      <c r="AM2" s="132"/>
-      <c r="AN2" s="134"/>
+      <c r="AL2" s="124"/>
+      <c r="AM2" s="146"/>
+      <c r="AN2" s="133"/>
       <c r="AO2" s="16"/>
       <c r="AP2" s="16"/>
       <c r="AQ2" s="16"/>
       <c r="AR2" s="16"/>
-      <c r="AS2" s="118"/>
-      <c r="AT2" s="120"/>
-      <c r="AU2" s="122"/>
-      <c r="AV2" s="124"/>
+      <c r="AS2" s="138"/>
+      <c r="AT2" s="140"/>
+      <c r="AU2" s="142"/>
+      <c r="AV2" s="144"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="74">
@@ -3183,7 +3209,7 @@
         <v>15</v>
       </c>
       <c r="AU3" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AV3" s="22"/>
     </row>
@@ -3241,7 +3267,7 @@
         <v>16</v>
       </c>
       <c r="AU4" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AV4" s="28"/>
     </row>
@@ -3299,7 +3325,7 @@
         <v>17</v>
       </c>
       <c r="AU5" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AV5" s="28"/>
     </row>
@@ -3357,7 +3383,7 @@
         <v>18</v>
       </c>
       <c r="AU6" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AV6" s="28"/>
     </row>
@@ -3410,12 +3436,11 @@
       <c r="AP7" s="24"/>
       <c r="AQ7" s="24"/>
       <c r="AR7" s="24"/>
-      <c r="AS7" s="24"/>
       <c r="AT7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="AU7" s="75" t="s">
-        <v>480</v>
+      <c r="AU7" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="AV7" s="28"/>
     </row>
@@ -3535,7 +3560,7 @@
         <v>1</v>
       </c>
       <c r="AU9" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AV9" s="28"/>
     </row>
@@ -4910,10 +4935,10 @@
       <c r="AR31" s="24"/>
       <c r="AS31" s="24"/>
       <c r="AT31" s="66" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AU31" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AV31" s="28"/>
     </row>
@@ -4976,10 +5001,10 @@
       <c r="AR32" s="24"/>
       <c r="AS32" s="24"/>
       <c r="AT32" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AU32" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AV32" s="28"/>
     </row>
@@ -5443,7 +5468,7 @@
         <v>32</v>
       </c>
       <c r="AU39" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AV39" s="28"/>
     </row>
@@ -5457,7 +5482,7 @@
       </c>
       <c r="D40" s="42"/>
       <c r="E40" s="43"/>
-      <c r="F40" s="55" t="s">
+      <c r="F40" s="41" t="s">
         <v>109</v>
       </c>
       <c r="G40" s="42"/>
@@ -5500,10 +5525,10 @@
       <c r="AR40" s="24"/>
       <c r="AS40" s="24"/>
       <c r="AT40" s="29" t="s">
-        <v>290</v>
+        <v>33</v>
       </c>
       <c r="AU40" s="2" t="s">
-        <v>292</v>
+        <v>237</v>
       </c>
       <c r="AV40" s="28"/>
     </row>
@@ -5980,10 +6005,10 @@
       <c r="AR48" s="24"/>
       <c r="AS48" s="24"/>
       <c r="AT48" s="29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AU48" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AV48" s="28"/>
     </row>
@@ -6046,10 +6071,10 @@
       <c r="AR49" s="24"/>
       <c r="AS49" s="24"/>
       <c r="AT49" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AU49" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AV49" s="28"/>
     </row>
@@ -6112,10 +6137,10 @@
       <c r="AR50" s="24"/>
       <c r="AS50" s="24"/>
       <c r="AT50" s="29" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AU50" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AV50" s="28"/>
     </row>
@@ -6297,7 +6322,7 @@
         <v>219</v>
       </c>
       <c r="AU53" s="66" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AV53" s="28"/>
     </row>
@@ -6363,7 +6388,7 @@
         <v>220</v>
       </c>
       <c r="AU54" s="66" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AV54" s="28"/>
     </row>
@@ -6429,7 +6454,7 @@
         <v>221</v>
       </c>
       <c r="AU55" s="66" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AV55" s="28"/>
     </row>
@@ -6491,7 +6516,7 @@
         <v>222</v>
       </c>
       <c r="AU56" s="66" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AV56" s="28"/>
     </row>
@@ -6548,10 +6573,10 @@
       <c r="AR57" s="24"/>
       <c r="AS57" s="24"/>
       <c r="AT57" s="29" t="s">
+        <v>483</v>
+      </c>
+      <c r="AU57" s="75" t="s">
         <v>484</v>
-      </c>
-      <c r="AU57" s="75" t="s">
-        <v>485</v>
       </c>
       <c r="AV57" s="28"/>
     </row>
@@ -7165,7 +7190,7 @@
         <v>58</v>
       </c>
       <c r="AU67" s="75" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AV67" s="28"/>
     </row>
@@ -7229,7 +7254,7 @@
         <v>59</v>
       </c>
       <c r="AU68" s="75" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AV68" s="28"/>
     </row>
@@ -7297,7 +7322,7 @@
         <v>60</v>
       </c>
       <c r="AU69" s="75" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AV69" s="28"/>
     </row>
@@ -7990,7 +8015,7 @@
       <c r="AR80" s="24"/>
       <c r="AS80" s="24"/>
       <c r="AT80" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AU80" s="29" t="s">
         <v>216</v>
@@ -8056,7 +8081,7 @@
       <c r="AR81" s="24"/>
       <c r="AS81" s="24"/>
       <c r="AT81" s="29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AU81" s="29" t="s">
         <v>216</v>
@@ -8122,7 +8147,7 @@
       <c r="AR82" s="24"/>
       <c r="AS82" s="24"/>
       <c r="AT82" s="29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AU82" s="29" t="s">
         <v>215</v>
@@ -8306,7 +8331,7 @@
       <c r="AR85" s="24"/>
       <c r="AS85" s="24"/>
       <c r="AT85" s="29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AU85" s="29" t="s">
         <v>215</v>
@@ -8369,7 +8394,7 @@
         <v>75</v>
       </c>
       <c r="AU86" s="29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AV86" s="28"/>
     </row>
@@ -8429,7 +8454,7 @@
         <v>76</v>
       </c>
       <c r="AU87" s="29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AV87" s="28"/>
     </row>
@@ -8609,7 +8634,7 @@
         <v>79</v>
       </c>
       <c r="AU90" s="29" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AV90" s="28"/>
     </row>
@@ -8874,8 +8899,8 @@
       <c r="AT94" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="AU94" s="29" t="s">
-        <v>230</v>
+      <c r="AU94" s="154" t="s">
+        <v>291</v>
       </c>
       <c r="AV94" s="28"/>
     </row>
@@ -8938,8 +8963,8 @@
       <c r="AT95" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="AU95" s="29" t="s">
-        <v>231</v>
+      <c r="AU95" s="75" t="s">
+        <v>479</v>
       </c>
       <c r="AV95" s="28"/>
     </row>
@@ -9035,7 +9060,7 @@
       <c r="Y97" s="24"/>
       <c r="Z97" s="24"/>
       <c r="AA97" s="25"/>
-      <c r="AB97" s="153" t="s">
+      <c r="AB97" s="117" t="s">
         <v>118</v>
       </c>
       <c r="AC97" s="27"/>
@@ -9060,10 +9085,10 @@
       <c r="AR97" s="24"/>
       <c r="AS97" s="24"/>
       <c r="AT97" s="66" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AU97" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AV97" s="28"/>
     </row>
@@ -9101,7 +9126,7 @@
       <c r="Y98" s="24"/>
       <c r="Z98" s="24"/>
       <c r="AA98" s="25"/>
-      <c r="AB98" s="153" t="s">
+      <c r="AB98" s="117" t="s">
         <v>117</v>
       </c>
       <c r="AC98" s="27"/>
@@ -9126,10 +9151,10 @@
       <c r="AR98" s="24"/>
       <c r="AS98" s="24"/>
       <c r="AT98" s="66" t="s">
+        <v>489</v>
+      </c>
+      <c r="AU98" s="4" t="s">
         <v>490</v>
-      </c>
-      <c r="AU98" s="4" t="s">
-        <v>491</v>
       </c>
       <c r="AV98" s="28"/>
     </row>
@@ -9188,8 +9213,8 @@
       <c r="AT99" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="AU99" s="2" t="s">
-        <v>232</v>
+      <c r="AU99" s="29" t="s">
+        <v>230</v>
       </c>
       <c r="AV99" s="28"/>
     </row>
@@ -9246,8 +9271,8 @@
       <c r="AT100" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="AU100" s="2" t="s">
-        <v>233</v>
+      <c r="AU100" s="29" t="s">
+        <v>231</v>
       </c>
       <c r="AV100" s="28"/>
     </row>
@@ -9359,10 +9384,10 @@
       <c r="AQ102" s="16"/>
       <c r="AR102" s="16"/>
       <c r="AS102" s="16"/>
-      <c r="AT102" s="45" t="s">
+      <c r="AT102" s="59" t="s">
         <v>263</v>
       </c>
-      <c r="AU102" s="45" t="s">
+      <c r="AU102" s="155" t="s">
         <v>263</v>
       </c>
       <c r="AV102" s="34"/>
@@ -9373,70 +9398,70 @@
       </c>
       <c r="B103" s="30"/>
       <c r="C103" s="30"/>
-      <c r="D103" s="145" t="s">
+      <c r="D103" s="122" t="s">
         <v>251</v>
       </c>
-      <c r="E103" s="145"/>
-      <c r="F103" s="145"/>
-      <c r="G103" s="145" t="s">
+      <c r="E103" s="122"/>
+      <c r="F103" s="122"/>
+      <c r="G103" s="122" t="s">
         <v>205</v>
       </c>
-      <c r="H103" s="145"/>
-      <c r="I103" s="145"/>
-      <c r="J103" s="145"/>
-      <c r="K103" s="145" t="s">
+      <c r="H103" s="122"/>
+      <c r="I103" s="122"/>
+      <c r="J103" s="122"/>
+      <c r="K103" s="122" t="s">
         <v>206</v>
       </c>
-      <c r="L103" s="145"/>
-      <c r="M103" s="145"/>
-      <c r="N103" s="145" t="s">
+      <c r="L103" s="122"/>
+      <c r="M103" s="122"/>
+      <c r="N103" s="122" t="s">
         <v>209</v>
       </c>
-      <c r="O103" s="145"/>
+      <c r="O103" s="122"/>
       <c r="P103" s="35" t="s">
         <v>283</v>
       </c>
       <c r="Q103" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="R103" s="144" t="s">
+      <c r="R103" s="121" t="s">
         <v>217</v>
       </c>
-      <c r="S103" s="144"/>
-      <c r="T103" s="144" t="s">
+      <c r="S103" s="121"/>
+      <c r="T103" s="121" t="s">
         <v>114</v>
       </c>
-      <c r="U103" s="144"/>
-      <c r="V103" s="145" t="s">
-        <v>488</v>
-      </c>
-      <c r="W103" s="145"/>
-      <c r="X103" s="145"/>
+      <c r="U103" s="121"/>
+      <c r="V103" s="122" t="s">
+        <v>487</v>
+      </c>
+      <c r="W103" s="122"/>
+      <c r="X103" s="122"/>
       <c r="Y103" s="35" t="s">
         <v>216</v>
       </c>
       <c r="Z103" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="AA103" s="144" t="s">
+      <c r="AA103" s="121" t="s">
         <v>218</v>
       </c>
-      <c r="AB103" s="144"/>
-      <c r="AC103" s="144"/>
-      <c r="AD103" s="144" t="s">
+      <c r="AB103" s="121"/>
+      <c r="AC103" s="121"/>
+      <c r="AD103" s="121" t="s">
         <v>224</v>
       </c>
-      <c r="AE103" s="144"/>
+      <c r="AE103" s="121"/>
       <c r="AF103" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="AG103" s="141"/>
-      <c r="AH103" s="141"/>
+      <c r="AG103" s="118"/>
+      <c r="AH103" s="118"/>
       <c r="AI103" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="AJ103" s="141"/>
-      <c r="AK103" s="141"/>
+      <c r="AJ103" s="118"/>
+      <c r="AK103" s="118"/>
       <c r="AL103" s="35" t="s">
         <v>129</v>
       </c>
@@ -9458,13 +9483,13 @@
       </c>
       <c r="AS103" s="30"/>
       <c r="AT103" s="30"/>
-      <c r="AU103" s="30"/>
+      <c r="AU103" s="156"/>
       <c r="AV103" s="30"/>
     </row>
     <row r="105" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B105" s="77"/>
       <c r="C105" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="106" spans="1:48" x14ac:dyDescent="0.25">
@@ -9472,25 +9497,25 @@
         <v>260</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="108" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="109" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="110" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="112" spans="1:48" ht="18" x14ac:dyDescent="0.35">
@@ -9498,7 +9523,7 @@
         <v>261</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -9506,7 +9531,7 @@
         <v>9</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -9514,11 +9539,31 @@
         <v>7</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="AS1:AS2"/>
+    <mergeCell ref="AT1:AT2"/>
+    <mergeCell ref="AU1:AU2"/>
+    <mergeCell ref="AV1:AV2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AN1:AN2"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:J1"/>
     <mergeCell ref="AG103:AH103"/>
     <mergeCell ref="AJ103:AK103"/>
     <mergeCell ref="B1:B2"/>
@@ -9535,26 +9580,6 @@
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="AS1:AS2"/>
-    <mergeCell ref="AT1:AT2"/>
-    <mergeCell ref="AU1:AU2"/>
-    <mergeCell ref="AV1:AV2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AM2"/>
-    <mergeCell ref="AN1:AN2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -9593,99 +9618,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="147" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="148"/>
+      <c r="C1" s="147" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="146" t="s">
-        <v>319</v>
-      </c>
-      <c r="D1" s="148"/>
-      <c r="E1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="150"/>
       <c r="F1" s="82" t="s">
-        <v>452</v>
-      </c>
-      <c r="G1" s="150" t="s">
+        <v>451</v>
+      </c>
+      <c r="G1" s="151" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="151"/>
-      <c r="K1" s="151"/>
-      <c r="L1" s="151"/>
-      <c r="M1" s="151"/>
-      <c r="N1" s="151"/>
-      <c r="O1" s="151"/>
-      <c r="P1" s="151"/>
-      <c r="Q1" s="151"/>
-      <c r="R1" s="151"/>
-      <c r="S1" s="151"/>
-      <c r="T1" s="151"/>
-      <c r="U1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="152"/>
+      <c r="J1" s="152"/>
+      <c r="K1" s="152"/>
+      <c r="L1" s="152"/>
+      <c r="M1" s="152"/>
+      <c r="N1" s="152"/>
+      <c r="O1" s="152"/>
+      <c r="P1" s="152"/>
+      <c r="Q1" s="152"/>
+      <c r="R1" s="152"/>
+      <c r="S1" s="152"/>
+      <c r="T1" s="152"/>
+      <c r="U1" s="153"/>
     </row>
     <row r="2" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="114" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="114" t="s">
+        <v>450</v>
+      </c>
+      <c r="C2" s="115" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="114" t="s">
+        <v>450</v>
+      </c>
+      <c r="E2" s="84" t="s">
         <v>320</v>
       </c>
-      <c r="B2" s="114" t="s">
-        <v>451</v>
-      </c>
-      <c r="C2" s="115" t="s">
-        <v>320</v>
-      </c>
-      <c r="D2" s="114" t="s">
-        <v>451</v>
-      </c>
-      <c r="E2" s="84" t="s">
+      <c r="F2" s="116" t="s">
+        <v>453</v>
+      </c>
+      <c r="G2" s="85" t="s">
         <v>321</v>
       </c>
-      <c r="F2" s="116" t="s">
-        <v>454</v>
-      </c>
-      <c r="G2" s="85" t="s">
+      <c r="H2" s="86" t="s">
         <v>322</v>
       </c>
-      <c r="H2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>323</v>
       </c>
-      <c r="I2" s="87" t="s">
+      <c r="J2" s="83" t="s">
         <v>324</v>
       </c>
-      <c r="J2" s="83" t="s">
-        <v>325</v>
-      </c>
       <c r="K2" s="114" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="L2" s="83" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="114" t="s">
+        <v>325</v>
+      </c>
+      <c r="N2" s="83" t="s">
         <v>326</v>
-      </c>
-      <c r="N2" s="83" t="s">
-        <v>327</v>
       </c>
       <c r="O2" s="83" t="s">
         <v>151</v>
       </c>
       <c r="P2" s="83" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q2" s="83" t="s">
         <v>328</v>
       </c>
-      <c r="Q2" s="83" t="s">
+      <c r="R2" s="83" t="s">
         <v>329</v>
       </c>
-      <c r="R2" s="83" t="s">
+      <c r="S2" s="83" t="s">
         <v>330</v>
       </c>
-      <c r="S2" s="83" t="s">
+      <c r="T2" s="83" t="s">
         <v>331</v>
       </c>
-      <c r="T2" s="83" t="s">
+      <c r="U2" s="88" t="s">
         <v>332</v>
-      </c>
-      <c r="U2" s="88" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -9693,7 +9718,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C3" s="89"/>
       <c r="E3" s="90"/>
@@ -9705,13 +9730,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C4" s="89">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E4" s="90"/>
       <c r="F4" s="91"/>
@@ -9722,22 +9747,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C5" s="89">
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E5" s="90" t="s">
         <v>336</v>
-      </c>
-      <c r="E5" s="90" t="s">
-        <v>337</v>
       </c>
       <c r="F5" s="91"/>
       <c r="G5" s="93"/>
       <c r="H5" s="94"/>
       <c r="I5" s="94" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J5" s="93"/>
       <c r="U5" s="92"/>
@@ -9747,13 +9772,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="95" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C6" s="96">
         <v>3</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E6" s="97"/>
       <c r="F6" s="98" t="s">
@@ -9770,10 +9795,10 @@
         <v>36</v>
       </c>
       <c r="M6" s="99" t="s">
+        <v>338</v>
+      </c>
+      <c r="N6" s="95" t="s">
         <v>339</v>
-      </c>
-      <c r="N6" s="95" t="s">
-        <v>340</v>
       </c>
       <c r="O6" s="95"/>
       <c r="P6" s="95"/>
@@ -9788,13 +9813,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="95" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C7" s="96">
         <v>4</v>
       </c>
       <c r="D7" s="95" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E7" s="97"/>
       <c r="F7" s="98" t="s">
@@ -9811,10 +9836,10 @@
         <v>39</v>
       </c>
       <c r="M7" s="99" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N7" s="95" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="O7" s="95"/>
       <c r="P7" s="95"/>
@@ -9829,13 +9854,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="95" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C8" s="96">
         <v>5</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E8" s="97"/>
       <c r="F8" s="98" t="s">
@@ -9852,10 +9877,10 @@
         <v>34</v>
       </c>
       <c r="M8" s="99" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N8" s="95" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="O8" s="95"/>
       <c r="P8" s="95"/>
@@ -9870,13 +9895,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="95" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C9" s="96">
         <v>6</v>
       </c>
       <c r="D9" s="95" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E9" s="97"/>
       <c r="F9" s="98" t="s">
@@ -9893,10 +9918,10 @@
         <v>35</v>
       </c>
       <c r="M9" s="99" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N9" s="95" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O9" s="95"/>
       <c r="P9" s="95"/>
@@ -9911,23 +9936,23 @@
         <v>8</v>
       </c>
       <c r="B10" s="102" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C10" s="103">
         <v>7</v>
       </c>
       <c r="D10" s="102" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E10" s="104"/>
       <c r="F10" s="105" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G10" s="106"/>
       <c r="H10" s="107"/>
       <c r="I10" s="107"/>
       <c r="J10" s="102" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K10" s="102">
         <v>9</v>
@@ -9937,11 +9962,11 @@
       </c>
       <c r="M10" s="102"/>
       <c r="N10" s="102" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="O10" s="102"/>
       <c r="P10" s="102" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q10" s="102"/>
       <c r="R10" s="102"/>
@@ -9954,23 +9979,23 @@
         <v>9</v>
       </c>
       <c r="B11" s="102" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C11" s="103">
         <v>8</v>
       </c>
       <c r="D11" s="102" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E11" s="104"/>
       <c r="F11" s="105" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G11" s="106"/>
       <c r="H11" s="107"/>
       <c r="I11" s="107"/>
       <c r="J11" s="102" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K11" s="102">
         <v>8</v>
@@ -9980,11 +10005,11 @@
       </c>
       <c r="M11" s="102"/>
       <c r="N11" s="102" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="O11" s="102"/>
       <c r="P11" s="102" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="Q11" s="102"/>
       <c r="R11" s="102"/>
@@ -9997,17 +10022,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="102" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C12" s="103">
         <v>9</v>
       </c>
       <c r="D12" s="102" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E12" s="104"/>
       <c r="F12" s="105" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G12" s="106"/>
       <c r="H12" s="107"/>
@@ -10021,10 +10046,10 @@
       </c>
       <c r="M12" s="102"/>
       <c r="N12" s="102" t="s">
+        <v>355</v>
+      </c>
+      <c r="O12" s="102" t="s">
         <v>356</v>
-      </c>
-      <c r="O12" s="102" t="s">
-        <v>357</v>
       </c>
       <c r="P12" s="102"/>
       <c r="Q12" s="102"/>
@@ -10032,7 +10057,7 @@
       <c r="S12" s="102"/>
       <c r="T12" s="102"/>
       <c r="U12" s="108" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -10040,17 +10065,17 @@
         <v>11</v>
       </c>
       <c r="B13" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C13" s="103">
         <v>10</v>
       </c>
       <c r="D13" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E13" s="104"/>
       <c r="F13" s="105" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G13" s="106"/>
       <c r="H13" s="107"/>
@@ -10064,10 +10089,10 @@
       </c>
       <c r="M13" s="102"/>
       <c r="N13" s="102" t="s">
+        <v>359</v>
+      </c>
+      <c r="O13" s="102" t="s">
         <v>360</v>
-      </c>
-      <c r="O13" s="102" t="s">
-        <v>361</v>
       </c>
       <c r="P13" s="102"/>
       <c r="Q13" s="102"/>
@@ -10075,7 +10100,7 @@
       <c r="S13" s="102"/>
       <c r="T13" s="102"/>
       <c r="U13" s="108" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -10083,17 +10108,17 @@
         <v>12</v>
       </c>
       <c r="B14" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C14" s="103">
         <v>11</v>
       </c>
       <c r="D14" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E14" s="104"/>
       <c r="F14" s="105" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G14" s="106"/>
       <c r="H14" s="107"/>
@@ -10107,18 +10132,18 @@
       </c>
       <c r="M14" s="102"/>
       <c r="N14" s="102" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O14" s="102"/>
       <c r="P14" s="102" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q14" s="102"/>
       <c r="R14" s="102"/>
       <c r="S14" s="102"/>
       <c r="T14" s="102"/>
       <c r="U14" s="108" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -10126,17 +10151,17 @@
         <v>13</v>
       </c>
       <c r="B15" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C15" s="103">
         <v>12</v>
       </c>
       <c r="D15" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E15" s="104"/>
       <c r="F15" s="105" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G15" s="106"/>
       <c r="H15" s="107"/>
@@ -10150,24 +10175,24 @@
       </c>
       <c r="M15" s="102"/>
       <c r="N15" s="102" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="O15" s="102"/>
       <c r="P15" s="102" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q15" s="102" t="s">
         <v>369</v>
       </c>
-      <c r="Q15" s="102" t="s">
+      <c r="R15" s="102" t="s">
         <v>370</v>
-      </c>
-      <c r="R15" s="102" t="s">
-        <v>371</v>
       </c>
       <c r="S15" s="102"/>
       <c r="T15" s="102" t="s">
+        <v>371</v>
+      </c>
+      <c r="U15" s="108" t="s">
         <v>372</v>
-      </c>
-      <c r="U15" s="108" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -10175,24 +10200,24 @@
         <v>14</v>
       </c>
       <c r="B16" s="102" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C16" s="103">
         <v>13</v>
       </c>
       <c r="D16" s="102" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E16" s="104"/>
       <c r="F16" s="105" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G16" s="106"/>
       <c r="H16" s="107" t="s">
+        <v>374</v>
+      </c>
+      <c r="I16" s="107" t="s">
         <v>375</v>
-      </c>
-      <c r="I16" s="107" t="s">
-        <v>376</v>
       </c>
       <c r="J16" s="106"/>
       <c r="K16" s="102">
@@ -10203,24 +10228,24 @@
       </c>
       <c r="M16" s="102"/>
       <c r="N16" s="102" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="O16" s="102"/>
       <c r="P16" s="102" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q16" s="102" t="s">
         <v>378</v>
       </c>
-      <c r="Q16" s="102" t="s">
+      <c r="R16" s="102" t="s">
         <v>379</v>
-      </c>
-      <c r="R16" s="102" t="s">
-        <v>380</v>
       </c>
       <c r="S16" s="102"/>
       <c r="T16" s="102" t="s">
+        <v>380</v>
+      </c>
+      <c r="U16" s="108" t="s">
         <v>381</v>
-      </c>
-      <c r="U16" s="108" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -10228,13 +10253,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C17" s="89">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E17" s="90"/>
       <c r="F17" s="91"/>
@@ -10245,17 +10270,17 @@
         <v>16</v>
       </c>
       <c r="B18" s="102" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C18" s="103">
         <v>15</v>
       </c>
       <c r="D18" s="102" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E18" s="104"/>
       <c r="F18" s="105" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G18" s="106"/>
       <c r="H18" s="107"/>
@@ -10269,24 +10294,24 @@
       </c>
       <c r="M18" s="102"/>
       <c r="N18" s="102" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="O18" s="102"/>
       <c r="P18" s="102" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q18" s="102" t="s">
         <v>385</v>
       </c>
-      <c r="Q18" s="102" t="s">
+      <c r="R18" s="102" t="s">
         <v>386</v>
-      </c>
-      <c r="R18" s="102" t="s">
-        <v>387</v>
       </c>
       <c r="S18" s="102"/>
       <c r="T18" s="102" t="s">
+        <v>387</v>
+      </c>
+      <c r="U18" s="108" t="s">
         <v>388</v>
-      </c>
-      <c r="U18" s="108" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -10294,18 +10319,18 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C19" s="89">
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E19" s="90"/>
       <c r="F19" s="91"/>
       <c r="G19" s="93" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H19" s="94"/>
       <c r="I19" s="94"/>
@@ -10314,10 +10339,10 @@
         <v>9</v>
       </c>
       <c r="R19" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="S19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="U19" s="92"/>
     </row>
@@ -10326,18 +10351,18 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C20" s="89">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E20" s="90"/>
       <c r="F20" s="91"/>
       <c r="G20" s="93" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H20" s="94"/>
       <c r="I20" s="94"/>
@@ -10346,10 +10371,10 @@
         <v>10</v>
       </c>
       <c r="R20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="S20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="U20" s="92"/>
     </row>
@@ -10369,7 +10394,7 @@
       <c r="E21" s="90"/>
       <c r="F21" s="91"/>
       <c r="G21" s="93" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H21" s="94"/>
       <c r="I21" s="94"/>
@@ -10378,7 +10403,7 @@
         <v>11</v>
       </c>
       <c r="R21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="S21" t="s">
         <v>176</v>
@@ -10390,7 +10415,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E22" s="90"/>
       <c r="F22" s="91"/>
@@ -10405,13 +10430,13 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C23" s="89">
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E23" s="90"/>
       <c r="F23" s="91"/>
@@ -10425,10 +10450,10 @@
         <v>6</v>
       </c>
       <c r="R23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="S23" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="U23" s="92"/>
     </row>
@@ -10437,13 +10462,13 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C24" s="89">
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E24" s="90"/>
       <c r="F24" s="91"/>
@@ -10457,10 +10482,10 @@
         <v>7</v>
       </c>
       <c r="R24" t="s">
+        <v>400</v>
+      </c>
+      <c r="S24" t="s">
         <v>401</v>
-      </c>
-      <c r="S24" t="s">
-        <v>402</v>
       </c>
       <c r="U24" s="92"/>
     </row>
@@ -10469,13 +10494,13 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C25" s="89">
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E25" s="90"/>
       <c r="F25" s="91"/>
@@ -10489,10 +10514,10 @@
         <v>8</v>
       </c>
       <c r="R25" t="s">
+        <v>403</v>
+      </c>
+      <c r="S25" t="s">
         <v>404</v>
-      </c>
-      <c r="S25" t="s">
-        <v>405</v>
       </c>
       <c r="U25" s="92"/>
     </row>
@@ -10501,24 +10526,24 @@
         <v>23</v>
       </c>
       <c r="B26" s="102" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C26" s="103">
         <v>23</v>
       </c>
       <c r="D26" s="102" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E26" s="107"/>
       <c r="F26" s="105" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G26" s="106"/>
       <c r="H26" s="107" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I26" s="107" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J26" s="106"/>
       <c r="K26" s="102">
@@ -10529,24 +10554,24 @@
       </c>
       <c r="M26" s="102"/>
       <c r="N26" s="102" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="O26" s="102"/>
       <c r="P26" s="102" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q26" s="102" t="s">
         <v>409</v>
       </c>
-      <c r="Q26" s="102" t="s">
+      <c r="R26" s="102" t="s">
         <v>410</v>
-      </c>
-      <c r="R26" s="102" t="s">
-        <v>411</v>
       </c>
       <c r="S26" s="102"/>
       <c r="T26" s="102" t="s">
         <v>176</v>
       </c>
       <c r="U26" s="108" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -10554,26 +10579,26 @@
         <v>24</v>
       </c>
       <c r="B27" s="102" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C27" s="103">
         <v>24</v>
       </c>
       <c r="D27" s="102" t="s">
+        <v>412</v>
+      </c>
+      <c r="E27" s="104" t="s">
         <v>413</v>
       </c>
-      <c r="E27" s="104" t="s">
-        <v>414</v>
-      </c>
       <c r="F27" s="105" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G27" s="106"/>
       <c r="H27" s="107" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I27" s="107" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J27" s="106"/>
       <c r="K27" s="102">
@@ -10584,19 +10609,19 @@
       </c>
       <c r="M27" s="102"/>
       <c r="N27" s="102" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="O27" s="102"/>
       <c r="P27" s="102" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q27" s="102"/>
       <c r="R27" s="102" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="S27" s="102"/>
       <c r="T27" s="102" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="U27" s="108"/>
     </row>
@@ -10605,26 +10630,26 @@
         <v>25</v>
       </c>
       <c r="B28" s="102" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C28" s="103">
         <v>25</v>
       </c>
       <c r="D28" s="102" t="s">
+        <v>418</v>
+      </c>
+      <c r="E28" s="104" t="s">
         <v>419</v>
       </c>
-      <c r="E28" s="104" t="s">
-        <v>420</v>
-      </c>
       <c r="F28" s="105" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G28" s="106"/>
       <c r="H28" s="107" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I28" s="107" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J28" s="106"/>
       <c r="K28" s="102">
@@ -10635,20 +10660,20 @@
       </c>
       <c r="M28" s="102"/>
       <c r="N28" s="102" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="O28" s="102"/>
       <c r="P28" s="102" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Q28" s="102"/>
       <c r="R28" s="102"/>
       <c r="S28" s="102"/>
       <c r="T28" s="102" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="U28" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -10656,17 +10681,17 @@
         <v>26</v>
       </c>
       <c r="B29" s="102" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C29" s="103">
         <v>26</v>
       </c>
       <c r="D29" s="102" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E29" s="104"/>
       <c r="F29" s="105" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G29" s="106"/>
       <c r="H29" s="107"/>
@@ -10680,20 +10705,20 @@
       </c>
       <c r="M29" s="102"/>
       <c r="N29" s="102" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O29" s="102"/>
       <c r="P29" s="102" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Q29" s="102"/>
       <c r="R29" s="102" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="S29" s="102"/>
       <c r="T29" s="102"/>
       <c r="U29" s="108" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -10701,17 +10726,17 @@
         <v>27</v>
       </c>
       <c r="B30" s="102" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C30" s="103">
         <v>27</v>
       </c>
       <c r="D30" s="102" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E30" s="104"/>
       <c r="F30" s="105" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G30" s="106"/>
       <c r="H30" s="107"/>
@@ -10730,7 +10755,7 @@
       <c r="S30" s="102"/>
       <c r="T30" s="102"/>
       <c r="U30" s="108" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -10738,17 +10763,17 @@
         <v>28</v>
       </c>
       <c r="B31" s="102" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C31" s="103">
         <v>28</v>
       </c>
       <c r="D31" s="102" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E31" s="104"/>
       <c r="F31" s="105" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G31" s="106"/>
       <c r="H31" s="107"/>
@@ -10767,7 +10792,7 @@
       <c r="S31" s="102"/>
       <c r="T31" s="102"/>
       <c r="U31" s="108" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -10775,24 +10800,24 @@
         <v>29</v>
       </c>
       <c r="B32" s="102" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C32" s="103">
         <v>29</v>
       </c>
       <c r="D32" s="102" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E32" s="104"/>
       <c r="F32" s="105" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G32" s="106"/>
       <c r="H32" s="107" t="s">
         <v>130</v>
       </c>
       <c r="I32" s="107" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J32" s="106"/>
       <c r="K32" s="102"/>
@@ -10805,12 +10830,12 @@
       <c r="P32" s="102"/>
       <c r="Q32" s="102"/>
       <c r="R32" s="102" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="S32" s="102"/>
       <c r="T32" s="102"/>
       <c r="U32" s="108" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -10818,17 +10843,17 @@
         <v>30</v>
       </c>
       <c r="B33" s="102" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C33" s="103">
         <v>30</v>
       </c>
       <c r="D33" s="102" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E33" s="104"/>
       <c r="F33" s="105" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G33" s="106"/>
       <c r="H33" s="107"/>
@@ -10844,7 +10869,7 @@
       <c r="P33" s="102"/>
       <c r="Q33" s="102"/>
       <c r="R33" s="102" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="S33" s="102"/>
       <c r="T33" s="102"/>
@@ -10855,17 +10880,17 @@
         <v>31</v>
       </c>
       <c r="B34" s="102" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C34" s="103">
         <v>31</v>
       </c>
       <c r="D34" s="102" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E34" s="104"/>
       <c r="F34" s="105" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G34" s="106"/>
       <c r="H34" s="107"/>
@@ -10881,12 +10906,12 @@
       <c r="P34" s="102"/>
       <c r="Q34" s="102"/>
       <c r="R34" s="102" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="S34" s="102"/>
       <c r="T34" s="102"/>
       <c r="U34" s="108" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -10911,17 +10936,17 @@
         <v>33</v>
       </c>
       <c r="B36" s="102" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C36" s="103">
         <v>33</v>
       </c>
       <c r="D36" s="102" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E36" s="104"/>
       <c r="F36" s="105" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G36" s="106"/>
       <c r="H36" s="107"/>
@@ -10937,12 +10962,12 @@
       <c r="P36" s="102"/>
       <c r="Q36" s="102"/>
       <c r="R36" s="102" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="S36" s="102"/>
       <c r="T36" s="102"/>
       <c r="U36" s="108" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -10950,17 +10975,17 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C37" s="89">
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E37" s="90"/>
       <c r="F37" s="91" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G37" s="93"/>
       <c r="H37" s="94"/>
@@ -10976,17 +11001,17 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C38" s="89">
         <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E38" s="90"/>
       <c r="F38" s="91" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G38" s="93"/>
       <c r="H38" s="94"/>
@@ -10996,7 +11021,7 @@
         <v>1</v>
       </c>
       <c r="U38" s="92" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -11004,17 +11029,17 @@
         <v>36</v>
       </c>
       <c r="B39" s="102" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C39" s="103">
         <v>36</v>
       </c>
       <c r="D39" s="102" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E39" s="104"/>
       <c r="F39" s="105" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G39" s="106"/>
       <c r="H39" s="107"/>
@@ -11030,12 +11055,12 @@
       <c r="P39" s="102"/>
       <c r="Q39" s="102"/>
       <c r="R39" s="102" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S39" s="102"/>
       <c r="T39" s="102"/>
       <c r="U39" s="108" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -11043,17 +11068,17 @@
         <v>37</v>
       </c>
       <c r="B40" s="102" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C40" s="103">
         <v>37</v>
       </c>
       <c r="D40" s="102" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E40" s="104"/>
       <c r="F40" s="105" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G40" s="106"/>
       <c r="H40" s="107"/>
@@ -11069,7 +11094,7 @@
       <c r="P40" s="102"/>
       <c r="Q40" s="102"/>
       <c r="R40" s="102" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="S40" s="102"/>
       <c r="T40" s="102"/>
@@ -11080,13 +11105,13 @@
         <v>38</v>
       </c>
       <c r="B41" s="109" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C41" s="110">
         <v>38</v>
       </c>
       <c r="D41" s="109" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E41" s="111"/>
       <c r="F41" s="112"/>
@@ -11109,18 +11134,18 @@
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="102"/>
       <c r="B43" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="95"/>
       <c r="B44" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MainBoard: Swap IN4A and IN4B, routed motors + servos
</commit_message>
<xml_diff>
--- a/ele/MainBoard/pinout.xlsx
+++ b/ele/MainBoard/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\RB3204-RBCX\ele\MainBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B2D46D-5FAD-42D6-8A1F-06D491B456FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608E7E89-D26D-415B-8828-AC4C14E38E48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{08978B24-E42F-429B-A3F9-EF8F7AA6C2ED}"/>
   </bookViews>
@@ -2479,57 +2479,11 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2554,12 +2508,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2581,11 +2586,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -2906,8 +2906,8 @@
   <dimension ref="A1:AV114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ96" sqref="AJ96"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AU85" sqref="AU85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,90 +2936,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="143" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="146" t="s">
         <v>259</v>
       </c>
       <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="129" t="s">
+      <c r="D1" s="139" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="131"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="129" t="s">
+      <c r="E1" s="140"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="139" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="129" t="s">
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="139" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="131"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="129" t="s">
+      <c r="L1" s="140"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="139" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="130"/>
-      <c r="P1" s="123" t="s">
+      <c r="O1" s="141"/>
+      <c r="P1" s="129" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="123" t="s">
+      <c r="Q1" s="129" t="s">
         <v>95</v>
       </c>
-      <c r="R1" s="125" t="s">
+      <c r="R1" s="131" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="126"/>
-      <c r="T1" s="125" t="s">
+      <c r="S1" s="132"/>
+      <c r="T1" s="131" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="126"/>
-      <c r="V1" s="129" t="s">
+      <c r="U1" s="132"/>
+      <c r="V1" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="W1" s="131"/>
-      <c r="X1" s="130"/>
-      <c r="Y1" s="123" t="s">
+      <c r="W1" s="140"/>
+      <c r="X1" s="141"/>
+      <c r="Y1" s="129" t="s">
         <v>306</v>
       </c>
-      <c r="Z1" s="123" t="s">
+      <c r="Z1" s="129" t="s">
         <v>307</v>
       </c>
-      <c r="AA1" s="125" t="s">
+      <c r="AA1" s="131" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="134"/>
-      <c r="AC1" s="126"/>
-      <c r="AD1" s="125" t="s">
+      <c r="AB1" s="142"/>
+      <c r="AC1" s="132"/>
+      <c r="AD1" s="131" t="s">
         <v>124</v>
       </c>
-      <c r="AE1" s="126"/>
+      <c r="AE1" s="132"/>
       <c r="AF1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="AG1" s="135" t="s">
+      <c r="AG1" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="AH1" s="136"/>
-      <c r="AI1" s="132" t="s">
+      <c r="AH1" s="134"/>
+      <c r="AI1" s="137" t="s">
         <v>126</v>
       </c>
-      <c r="AJ1" s="135" t="s">
+      <c r="AJ1" s="133" t="s">
         <v>127</v>
       </c>
-      <c r="AK1" s="136"/>
-      <c r="AL1" s="123" t="s">
+      <c r="AK1" s="134"/>
+      <c r="AL1" s="129" t="s">
         <v>129</v>
       </c>
-      <c r="AM1" s="145" t="s">
+      <c r="AM1" s="135" t="s">
         <v>130</v>
       </c>
-      <c r="AN1" s="132" t="s">
+      <c r="AN1" s="137" t="s">
         <v>151</v>
       </c>
       <c r="AO1" s="8" t="s">
@@ -3034,22 +3034,22 @@
       <c r="AR1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="AS1" s="137" t="s">
+      <c r="AS1" s="121" t="s">
         <v>141</v>
       </c>
-      <c r="AT1" s="139" t="s">
+      <c r="AT1" s="123" t="s">
         <v>182</v>
       </c>
-      <c r="AU1" s="141" t="s">
+      <c r="AU1" s="125" t="s">
         <v>183</v>
       </c>
-      <c r="AV1" s="143" t="s">
+      <c r="AV1" s="127" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="128"/>
-      <c r="B2" s="120"/>
+      <c r="A2" s="144"/>
+      <c r="B2" s="147"/>
       <c r="C2" s="37" t="s">
         <v>96</v>
       </c>
@@ -3089,8 +3089,8 @@
       <c r="O2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
+      <c r="P2" s="130"/>
+      <c r="Q2" s="130"/>
       <c r="R2" s="9" t="s">
         <v>105</v>
       </c>
@@ -3112,8 +3112,8 @@
       <c r="X2" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="Y2" s="124"/>
-      <c r="Z2" s="124"/>
+      <c r="Y2" s="130"/>
+      <c r="Z2" s="130"/>
       <c r="AA2" s="9" t="s">
         <v>101</v>
       </c>
@@ -3136,24 +3136,24 @@
       <c r="AH2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AI2" s="133"/>
+      <c r="AI2" s="138"/>
       <c r="AJ2" s="9" t="s">
         <v>105</v>
       </c>
       <c r="AK2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AL2" s="124"/>
-      <c r="AM2" s="146"/>
-      <c r="AN2" s="133"/>
+      <c r="AL2" s="130"/>
+      <c r="AM2" s="136"/>
+      <c r="AN2" s="138"/>
       <c r="AO2" s="16"/>
       <c r="AP2" s="16"/>
       <c r="AQ2" s="16"/>
       <c r="AR2" s="16"/>
-      <c r="AS2" s="138"/>
-      <c r="AT2" s="140"/>
-      <c r="AU2" s="142"/>
-      <c r="AV2" s="144"/>
+      <c r="AS2" s="122"/>
+      <c r="AT2" s="124"/>
+      <c r="AU2" s="126"/>
+      <c r="AV2" s="128"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="74">
@@ -8210,7 +8210,7 @@
         <v>72</v>
       </c>
       <c r="AU83" s="29" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AV83" s="28"/>
     </row>
@@ -8270,7 +8270,7 @@
         <v>73</v>
       </c>
       <c r="AU84" s="29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AV84" s="28"/>
     </row>
@@ -8899,7 +8899,7 @@
       <c r="AT94" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="AU94" s="154" t="s">
+      <c r="AU94" s="118" t="s">
         <v>291</v>
       </c>
       <c r="AV94" s="28"/>
@@ -9387,7 +9387,7 @@
       <c r="AT102" s="59" t="s">
         <v>263</v>
       </c>
-      <c r="AU102" s="155" t="s">
+      <c r="AU102" s="119" t="s">
         <v>263</v>
       </c>
       <c r="AV102" s="34"/>
@@ -9398,70 +9398,70 @@
       </c>
       <c r="B103" s="30"/>
       <c r="C103" s="30"/>
-      <c r="D103" s="122" t="s">
+      <c r="D103" s="149" t="s">
         <v>251</v>
       </c>
-      <c r="E103" s="122"/>
-      <c r="F103" s="122"/>
-      <c r="G103" s="122" t="s">
+      <c r="E103" s="149"/>
+      <c r="F103" s="149"/>
+      <c r="G103" s="149" t="s">
         <v>205</v>
       </c>
-      <c r="H103" s="122"/>
-      <c r="I103" s="122"/>
-      <c r="J103" s="122"/>
-      <c r="K103" s="122" t="s">
+      <c r="H103" s="149"/>
+      <c r="I103" s="149"/>
+      <c r="J103" s="149"/>
+      <c r="K103" s="149" t="s">
         <v>206</v>
       </c>
-      <c r="L103" s="122"/>
-      <c r="M103" s="122"/>
-      <c r="N103" s="122" t="s">
+      <c r="L103" s="149"/>
+      <c r="M103" s="149"/>
+      <c r="N103" s="149" t="s">
         <v>209</v>
       </c>
-      <c r="O103" s="122"/>
+      <c r="O103" s="149"/>
       <c r="P103" s="35" t="s">
         <v>283</v>
       </c>
       <c r="Q103" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="R103" s="121" t="s">
+      <c r="R103" s="148" t="s">
         <v>217</v>
       </c>
-      <c r="S103" s="121"/>
-      <c r="T103" s="121" t="s">
+      <c r="S103" s="148"/>
+      <c r="T103" s="148" t="s">
         <v>114</v>
       </c>
-      <c r="U103" s="121"/>
-      <c r="V103" s="122" t="s">
+      <c r="U103" s="148"/>
+      <c r="V103" s="149" t="s">
         <v>487</v>
       </c>
-      <c r="W103" s="122"/>
-      <c r="X103" s="122"/>
+      <c r="W103" s="149"/>
+      <c r="X103" s="149"/>
       <c r="Y103" s="35" t="s">
         <v>216</v>
       </c>
       <c r="Z103" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="AA103" s="121" t="s">
+      <c r="AA103" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="AB103" s="121"/>
-      <c r="AC103" s="121"/>
-      <c r="AD103" s="121" t="s">
+      <c r="AB103" s="148"/>
+      <c r="AC103" s="148"/>
+      <c r="AD103" s="148" t="s">
         <v>224</v>
       </c>
-      <c r="AE103" s="121"/>
+      <c r="AE103" s="148"/>
       <c r="AF103" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="AG103" s="118"/>
-      <c r="AH103" s="118"/>
+      <c r="AG103" s="145"/>
+      <c r="AH103" s="145"/>
       <c r="AI103" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="AJ103" s="118"/>
-      <c r="AK103" s="118"/>
+      <c r="AJ103" s="145"/>
+      <c r="AK103" s="145"/>
       <c r="AL103" s="35" t="s">
         <v>129</v>
       </c>
@@ -9483,7 +9483,7 @@
       </c>
       <c r="AS103" s="30"/>
       <c r="AT103" s="30"/>
-      <c r="AU103" s="156"/>
+      <c r="AU103" s="120"/>
       <c r="AV103" s="30"/>
     </row>
     <row r="105" spans="1:48" x14ac:dyDescent="0.25">
@@ -9544,26 +9544,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="AS1:AS2"/>
-    <mergeCell ref="AT1:AT2"/>
-    <mergeCell ref="AU1:AU2"/>
-    <mergeCell ref="AV1:AV2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AM2"/>
-    <mergeCell ref="AN1:AN2"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:J1"/>
     <mergeCell ref="AG103:AH103"/>
     <mergeCell ref="AJ103:AK103"/>
     <mergeCell ref="B1:B2"/>
@@ -9580,6 +9560,26 @@
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="AS1:AS2"/>
+    <mergeCell ref="AT1:AT2"/>
+    <mergeCell ref="AU1:AU2"/>
+    <mergeCell ref="AV1:AV2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AN1:AN2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -9618,35 +9618,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="150" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="147" t="s">
+      <c r="B1" s="151"/>
+      <c r="C1" s="150" t="s">
         <v>318</v>
       </c>
-      <c r="D1" s="149"/>
-      <c r="E1" s="150"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="153"/>
       <c r="F1" s="82" t="s">
         <v>451</v>
       </c>
-      <c r="G1" s="151" t="s">
+      <c r="G1" s="154" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="152"/>
-      <c r="K1" s="152"/>
-      <c r="L1" s="152"/>
-      <c r="M1" s="152"/>
-      <c r="N1" s="152"/>
-      <c r="O1" s="152"/>
-      <c r="P1" s="152"/>
-      <c r="Q1" s="152"/>
-      <c r="R1" s="152"/>
-      <c r="S1" s="152"/>
-      <c r="T1" s="152"/>
-      <c r="U1" s="153"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="155"/>
+      <c r="J1" s="155"/>
+      <c r="K1" s="155"/>
+      <c r="L1" s="155"/>
+      <c r="M1" s="155"/>
+      <c r="N1" s="155"/>
+      <c r="O1" s="155"/>
+      <c r="P1" s="155"/>
+      <c r="Q1" s="155"/>
+      <c r="R1" s="155"/>
+      <c r="S1" s="155"/>
+      <c r="T1" s="155"/>
+      <c r="U1" s="156"/>
     </row>
     <row r="2" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="114" t="s">

</xml_diff>

<commit_message>
MainBoard: Compete USB, swap VUSB_DET and BUTTON_ON, all parts on board
</commit_message>
<xml_diff>
--- a/ele/MainBoard/pinout.xlsx
+++ b/ele/MainBoard/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\RB3204-RBCX\ele\MainBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608E7E89-D26D-415B-8828-AC4C14E38E48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CC2F07-2096-4EC7-B468-F7AF9F567D33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{08978B24-E42F-429B-A3F9-EF8F7AA6C2ED}"/>
   </bookViews>
@@ -1014,9 +1014,6 @@
     <t>BUTTON4</t>
   </si>
   <si>
-    <t>BUTTON_ENTER/ON</t>
-  </si>
-  <si>
     <t>BUTTON_ESC/OFF</t>
   </si>
   <si>
@@ -1603,6 +1600,9 @@
   </si>
   <si>
     <t>CAN/I2C</t>
+  </si>
+  <si>
+    <t>BUTTON_ON</t>
   </si>
 </sst>
 </file>
@@ -2484,6 +2484,57 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2508,63 +2559,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2905,9 +2905,9 @@
   </sheetPr>
   <dimension ref="A1:AV114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AU85" sqref="AU85"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AU10" sqref="AU10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,90 +2936,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="130" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="122" t="s">
         <v>259</v>
       </c>
       <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="139" t="s">
+      <c r="D1" s="132" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="140"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="139" t="s">
+      <c r="E1" s="134"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="132" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="141"/>
-      <c r="K1" s="139" t="s">
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="132" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="140"/>
-      <c r="M1" s="141"/>
-      <c r="N1" s="139" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="132" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="141"/>
-      <c r="P1" s="129" t="s">
+      <c r="O1" s="133"/>
+      <c r="P1" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="129" t="s">
+      <c r="Q1" s="126" t="s">
         <v>95</v>
       </c>
-      <c r="R1" s="131" t="s">
+      <c r="R1" s="128" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="132"/>
-      <c r="T1" s="131" t="s">
+      <c r="S1" s="129"/>
+      <c r="T1" s="128" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="132"/>
-      <c r="V1" s="139" t="s">
+      <c r="U1" s="129"/>
+      <c r="V1" s="132" t="s">
         <v>116</v>
       </c>
-      <c r="W1" s="140"/>
-      <c r="X1" s="141"/>
-      <c r="Y1" s="129" t="s">
+      <c r="W1" s="134"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="126" t="s">
+        <v>305</v>
+      </c>
+      <c r="Z1" s="126" t="s">
         <v>306</v>
       </c>
-      <c r="Z1" s="129" t="s">
-        <v>307</v>
-      </c>
-      <c r="AA1" s="131" t="s">
+      <c r="AA1" s="128" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="142"/>
-      <c r="AC1" s="132"/>
-      <c r="AD1" s="131" t="s">
+      <c r="AB1" s="137"/>
+      <c r="AC1" s="129"/>
+      <c r="AD1" s="128" t="s">
         <v>124</v>
       </c>
-      <c r="AE1" s="132"/>
+      <c r="AE1" s="129"/>
       <c r="AF1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="AG1" s="133" t="s">
+      <c r="AG1" s="138" t="s">
         <v>125</v>
       </c>
-      <c r="AH1" s="134"/>
-      <c r="AI1" s="137" t="s">
+      <c r="AH1" s="139"/>
+      <c r="AI1" s="135" t="s">
         <v>126</v>
       </c>
-      <c r="AJ1" s="133" t="s">
+      <c r="AJ1" s="138" t="s">
         <v>127</v>
       </c>
-      <c r="AK1" s="134"/>
-      <c r="AL1" s="129" t="s">
+      <c r="AK1" s="139"/>
+      <c r="AL1" s="126" t="s">
         <v>129</v>
       </c>
-      <c r="AM1" s="135" t="s">
+      <c r="AM1" s="148" t="s">
         <v>130</v>
       </c>
-      <c r="AN1" s="137" t="s">
+      <c r="AN1" s="135" t="s">
         <v>151</v>
       </c>
       <c r="AO1" s="8" t="s">
@@ -3034,22 +3034,22 @@
       <c r="AR1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="AS1" s="121" t="s">
+      <c r="AS1" s="140" t="s">
         <v>141</v>
       </c>
-      <c r="AT1" s="123" t="s">
+      <c r="AT1" s="142" t="s">
         <v>182</v>
       </c>
-      <c r="AU1" s="125" t="s">
+      <c r="AU1" s="144" t="s">
         <v>183</v>
       </c>
-      <c r="AV1" s="127" t="s">
+      <c r="AV1" s="146" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="144"/>
-      <c r="B2" s="147"/>
+      <c r="A2" s="131"/>
+      <c r="B2" s="123"/>
       <c r="C2" s="37" t="s">
         <v>96</v>
       </c>
@@ -3089,8 +3089,8 @@
       <c r="O2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="130"/>
-      <c r="Q2" s="130"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
       <c r="R2" s="9" t="s">
         <v>105</v>
       </c>
@@ -3112,8 +3112,8 @@
       <c r="X2" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="Y2" s="130"/>
-      <c r="Z2" s="130"/>
+      <c r="Y2" s="127"/>
+      <c r="Z2" s="127"/>
       <c r="AA2" s="9" t="s">
         <v>101</v>
       </c>
@@ -3136,24 +3136,24 @@
       <c r="AH2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AI2" s="138"/>
+      <c r="AI2" s="136"/>
       <c r="AJ2" s="9" t="s">
         <v>105</v>
       </c>
       <c r="AK2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AL2" s="130"/>
-      <c r="AM2" s="136"/>
-      <c r="AN2" s="138"/>
+      <c r="AL2" s="127"/>
+      <c r="AM2" s="149"/>
+      <c r="AN2" s="136"/>
       <c r="AO2" s="16"/>
       <c r="AP2" s="16"/>
       <c r="AQ2" s="16"/>
       <c r="AR2" s="16"/>
-      <c r="AS2" s="122"/>
-      <c r="AT2" s="124"/>
-      <c r="AU2" s="126"/>
-      <c r="AV2" s="128"/>
+      <c r="AS2" s="141"/>
+      <c r="AT2" s="143"/>
+      <c r="AU2" s="145"/>
+      <c r="AV2" s="147"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="74">
@@ -3560,7 +3560,7 @@
         <v>1</v>
       </c>
       <c r="AU9" s="2" t="s">
-        <v>294</v>
+        <v>484</v>
       </c>
       <c r="AV9" s="28"/>
     </row>
@@ -4935,10 +4935,10 @@
       <c r="AR31" s="24"/>
       <c r="AS31" s="24"/>
       <c r="AT31" s="66" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AU31" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AV31" s="28"/>
     </row>
@@ -5001,10 +5001,10 @@
       <c r="AR32" s="24"/>
       <c r="AS32" s="24"/>
       <c r="AT32" s="66" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AU32" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AV32" s="28"/>
     </row>
@@ -6008,7 +6008,7 @@
         <v>290</v>
       </c>
       <c r="AU48" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AV48" s="28"/>
     </row>
@@ -6071,10 +6071,10 @@
       <c r="AR49" s="24"/>
       <c r="AS49" s="24"/>
       <c r="AT49" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AU49" s="29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AV49" s="28"/>
     </row>
@@ -6137,10 +6137,10 @@
       <c r="AR50" s="24"/>
       <c r="AS50" s="24"/>
       <c r="AT50" s="29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AU50" s="29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AV50" s="28"/>
     </row>
@@ -6322,7 +6322,7 @@
         <v>219</v>
       </c>
       <c r="AU53" s="66" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AV53" s="28"/>
     </row>
@@ -6388,7 +6388,7 @@
         <v>220</v>
       </c>
       <c r="AU54" s="66" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AV54" s="28"/>
     </row>
@@ -6454,7 +6454,7 @@
         <v>221</v>
       </c>
       <c r="AU55" s="66" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AV55" s="28"/>
     </row>
@@ -6516,7 +6516,7 @@
         <v>222</v>
       </c>
       <c r="AU56" s="66" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AV56" s="28"/>
     </row>
@@ -6573,10 +6573,10 @@
       <c r="AR57" s="24"/>
       <c r="AS57" s="24"/>
       <c r="AT57" s="29" t="s">
+        <v>482</v>
+      </c>
+      <c r="AU57" s="75" t="s">
         <v>483</v>
-      </c>
-      <c r="AU57" s="75" t="s">
-        <v>484</v>
       </c>
       <c r="AV57" s="28"/>
     </row>
@@ -7190,7 +7190,7 @@
         <v>58</v>
       </c>
       <c r="AU67" s="75" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AV67" s="28"/>
     </row>
@@ -7254,7 +7254,7 @@
         <v>59</v>
       </c>
       <c r="AU68" s="75" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="AV68" s="28"/>
     </row>
@@ -7322,7 +7322,7 @@
         <v>60</v>
       </c>
       <c r="AU69" s="75" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AV69" s="28"/>
     </row>
@@ -8015,7 +8015,7 @@
       <c r="AR80" s="24"/>
       <c r="AS80" s="24"/>
       <c r="AT80" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AU80" s="29" t="s">
         <v>216</v>
@@ -8081,7 +8081,7 @@
       <c r="AR81" s="24"/>
       <c r="AS81" s="24"/>
       <c r="AT81" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AU81" s="29" t="s">
         <v>216</v>
@@ -8147,7 +8147,7 @@
       <c r="AR82" s="24"/>
       <c r="AS82" s="24"/>
       <c r="AT82" s="29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AU82" s="29" t="s">
         <v>215</v>
@@ -8331,7 +8331,7 @@
       <c r="AR85" s="24"/>
       <c r="AS85" s="24"/>
       <c r="AT85" s="29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AU85" s="29" t="s">
         <v>215</v>
@@ -8394,7 +8394,7 @@
         <v>75</v>
       </c>
       <c r="AU86" s="29" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AV86" s="28"/>
     </row>
@@ -8634,7 +8634,7 @@
         <v>79</v>
       </c>
       <c r="AU90" s="29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AV90" s="28"/>
     </row>
@@ -8964,7 +8964,7 @@
         <v>84</v>
       </c>
       <c r="AU95" s="75" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AV95" s="28"/>
     </row>
@@ -9085,10 +9085,10 @@
       <c r="AR97" s="24"/>
       <c r="AS97" s="24"/>
       <c r="AT97" s="66" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AU97" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AV97" s="28"/>
     </row>
@@ -9151,10 +9151,10 @@
       <c r="AR98" s="24"/>
       <c r="AS98" s="24"/>
       <c r="AT98" s="66" t="s">
+        <v>488</v>
+      </c>
+      <c r="AU98" s="4" t="s">
         <v>489</v>
-      </c>
-      <c r="AU98" s="4" t="s">
-        <v>490</v>
       </c>
       <c r="AV98" s="28"/>
     </row>
@@ -9398,70 +9398,70 @@
       </c>
       <c r="B103" s="30"/>
       <c r="C103" s="30"/>
-      <c r="D103" s="149" t="s">
+      <c r="D103" s="125" t="s">
         <v>251</v>
       </c>
-      <c r="E103" s="149"/>
-      <c r="F103" s="149"/>
-      <c r="G103" s="149" t="s">
+      <c r="E103" s="125"/>
+      <c r="F103" s="125"/>
+      <c r="G103" s="125" t="s">
         <v>205</v>
       </c>
-      <c r="H103" s="149"/>
-      <c r="I103" s="149"/>
-      <c r="J103" s="149"/>
-      <c r="K103" s="149" t="s">
+      <c r="H103" s="125"/>
+      <c r="I103" s="125"/>
+      <c r="J103" s="125"/>
+      <c r="K103" s="125" t="s">
         <v>206</v>
       </c>
-      <c r="L103" s="149"/>
-      <c r="M103" s="149"/>
-      <c r="N103" s="149" t="s">
+      <c r="L103" s="125"/>
+      <c r="M103" s="125"/>
+      <c r="N103" s="125" t="s">
         <v>209</v>
       </c>
-      <c r="O103" s="149"/>
+      <c r="O103" s="125"/>
       <c r="P103" s="35" t="s">
         <v>283</v>
       </c>
       <c r="Q103" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="R103" s="148" t="s">
+      <c r="R103" s="124" t="s">
         <v>217</v>
       </c>
-      <c r="S103" s="148"/>
-      <c r="T103" s="148" t="s">
+      <c r="S103" s="124"/>
+      <c r="T103" s="124" t="s">
         <v>114</v>
       </c>
-      <c r="U103" s="148"/>
-      <c r="V103" s="149" t="s">
-        <v>487</v>
-      </c>
-      <c r="W103" s="149"/>
-      <c r="X103" s="149"/>
+      <c r="U103" s="124"/>
+      <c r="V103" s="125" t="s">
+        <v>486</v>
+      </c>
+      <c r="W103" s="125"/>
+      <c r="X103" s="125"/>
       <c r="Y103" s="35" t="s">
         <v>216</v>
       </c>
       <c r="Z103" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="AA103" s="148" t="s">
+      <c r="AA103" s="124" t="s">
         <v>218</v>
       </c>
-      <c r="AB103" s="148"/>
-      <c r="AC103" s="148"/>
-      <c r="AD103" s="148" t="s">
+      <c r="AB103" s="124"/>
+      <c r="AC103" s="124"/>
+      <c r="AD103" s="124" t="s">
         <v>224</v>
       </c>
-      <c r="AE103" s="148"/>
+      <c r="AE103" s="124"/>
       <c r="AF103" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="AG103" s="145"/>
-      <c r="AH103" s="145"/>
+      <c r="AG103" s="121"/>
+      <c r="AH103" s="121"/>
       <c r="AI103" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="AJ103" s="145"/>
-      <c r="AK103" s="145"/>
+      <c r="AJ103" s="121"/>
+      <c r="AK103" s="121"/>
       <c r="AL103" s="35" t="s">
         <v>129</v>
       </c>
@@ -9489,7 +9489,7 @@
     <row r="105" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B105" s="77"/>
       <c r="C105" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="106" spans="1:48" x14ac:dyDescent="0.25">
@@ -9497,25 +9497,25 @@
         <v>260</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="109" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="110" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="112" spans="1:48" ht="18" x14ac:dyDescent="0.35">
@@ -9523,7 +9523,7 @@
         <v>261</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -9531,7 +9531,7 @@
         <v>9</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -9539,11 +9539,31 @@
         <v>7</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="AS1:AS2"/>
+    <mergeCell ref="AT1:AT2"/>
+    <mergeCell ref="AU1:AU2"/>
+    <mergeCell ref="AV1:AV2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AN1:AN2"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:J1"/>
     <mergeCell ref="AG103:AH103"/>
     <mergeCell ref="AJ103:AK103"/>
     <mergeCell ref="B1:B2"/>
@@ -9560,26 +9580,6 @@
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="AS1:AS2"/>
-    <mergeCell ref="AT1:AT2"/>
-    <mergeCell ref="AU1:AU2"/>
-    <mergeCell ref="AV1:AV2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AM2"/>
-    <mergeCell ref="AN1:AN2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -9619,16 +9619,16 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="150" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B1" s="151"/>
       <c r="C1" s="150" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D1" s="152"/>
       <c r="E1" s="153"/>
       <c r="F1" s="82" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G1" s="154" t="s">
         <v>182</v>
@@ -9650,67 +9650,67 @@
     </row>
     <row r="2" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="114" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="114" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" s="115" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" s="114" t="s">
+        <v>449</v>
+      </c>
+      <c r="E2" s="84" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="114" t="s">
-        <v>450</v>
-      </c>
-      <c r="C2" s="115" t="s">
-        <v>319</v>
-      </c>
-      <c r="D2" s="114" t="s">
-        <v>450</v>
-      </c>
-      <c r="E2" s="84" t="s">
+      <c r="F2" s="116" t="s">
+        <v>452</v>
+      </c>
+      <c r="G2" s="85" t="s">
         <v>320</v>
       </c>
-      <c r="F2" s="116" t="s">
-        <v>453</v>
-      </c>
-      <c r="G2" s="85" t="s">
+      <c r="H2" s="86" t="s">
         <v>321</v>
       </c>
-      <c r="H2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>322</v>
       </c>
-      <c r="I2" s="87" t="s">
+      <c r="J2" s="83" t="s">
         <v>323</v>
       </c>
-      <c r="J2" s="83" t="s">
-        <v>324</v>
-      </c>
       <c r="K2" s="114" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L2" s="83" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="114" t="s">
+        <v>324</v>
+      </c>
+      <c r="N2" s="83" t="s">
         <v>325</v>
-      </c>
-      <c r="N2" s="83" t="s">
-        <v>326</v>
       </c>
       <c r="O2" s="83" t="s">
         <v>151</v>
       </c>
       <c r="P2" s="83" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q2" s="83" t="s">
         <v>327</v>
       </c>
-      <c r="Q2" s="83" t="s">
+      <c r="R2" s="83" t="s">
         <v>328</v>
       </c>
-      <c r="R2" s="83" t="s">
+      <c r="S2" s="83" t="s">
         <v>329</v>
       </c>
-      <c r="S2" s="83" t="s">
+      <c r="T2" s="83" t="s">
         <v>330</v>
       </c>
-      <c r="T2" s="83" t="s">
+      <c r="U2" s="88" t="s">
         <v>331</v>
-      </c>
-      <c r="U2" s="88" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -9718,7 +9718,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C3" s="89"/>
       <c r="E3" s="90"/>
@@ -9730,13 +9730,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C4" s="89">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E4" s="90"/>
       <c r="F4" s="91"/>
@@ -9747,22 +9747,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C5" s="89">
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E5" s="90" t="s">
         <v>335</v>
-      </c>
-      <c r="E5" s="90" t="s">
-        <v>336</v>
       </c>
       <c r="F5" s="91"/>
       <c r="G5" s="93"/>
       <c r="H5" s="94"/>
       <c r="I5" s="94" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J5" s="93"/>
       <c r="U5" s="92"/>
@@ -9772,13 +9772,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="95" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C6" s="96">
         <v>3</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E6" s="97"/>
       <c r="F6" s="98" t="s">
@@ -9795,10 +9795,10 @@
         <v>36</v>
       </c>
       <c r="M6" s="99" t="s">
+        <v>337</v>
+      </c>
+      <c r="N6" s="95" t="s">
         <v>338</v>
-      </c>
-      <c r="N6" s="95" t="s">
-        <v>339</v>
       </c>
       <c r="O6" s="95"/>
       <c r="P6" s="95"/>
@@ -9813,13 +9813,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="95" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C7" s="96">
         <v>4</v>
       </c>
       <c r="D7" s="95" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E7" s="97"/>
       <c r="F7" s="98" t="s">
@@ -9836,10 +9836,10 @@
         <v>39</v>
       </c>
       <c r="M7" s="99" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N7" s="95" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O7" s="95"/>
       <c r="P7" s="95"/>
@@ -9854,13 +9854,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="95" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C8" s="96">
         <v>5</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E8" s="97"/>
       <c r="F8" s="98" t="s">
@@ -9877,10 +9877,10 @@
         <v>34</v>
       </c>
       <c r="M8" s="99" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N8" s="95" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="O8" s="95"/>
       <c r="P8" s="95"/>
@@ -9895,13 +9895,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="95" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C9" s="96">
         <v>6</v>
       </c>
       <c r="D9" s="95" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E9" s="97"/>
       <c r="F9" s="98" t="s">
@@ -9918,10 +9918,10 @@
         <v>35</v>
       </c>
       <c r="M9" s="99" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N9" s="95" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="O9" s="95"/>
       <c r="P9" s="95"/>
@@ -9936,23 +9936,23 @@
         <v>8</v>
       </c>
       <c r="B10" s="102" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C10" s="103">
         <v>7</v>
       </c>
       <c r="D10" s="102" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E10" s="104"/>
       <c r="F10" s="105" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G10" s="106"/>
       <c r="H10" s="107"/>
       <c r="I10" s="107"/>
       <c r="J10" s="102" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K10" s="102">
         <v>9</v>
@@ -9962,11 +9962,11 @@
       </c>
       <c r="M10" s="102"/>
       <c r="N10" s="102" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O10" s="102"/>
       <c r="P10" s="102" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q10" s="102"/>
       <c r="R10" s="102"/>
@@ -9979,23 +9979,23 @@
         <v>9</v>
       </c>
       <c r="B11" s="102" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C11" s="103">
         <v>8</v>
       </c>
       <c r="D11" s="102" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E11" s="104"/>
       <c r="F11" s="105" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G11" s="106"/>
       <c r="H11" s="107"/>
       <c r="I11" s="107"/>
       <c r="J11" s="102" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K11" s="102">
         <v>8</v>
@@ -10005,11 +10005,11 @@
       </c>
       <c r="M11" s="102"/>
       <c r="N11" s="102" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O11" s="102"/>
       <c r="P11" s="102" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q11" s="102"/>
       <c r="R11" s="102"/>
@@ -10022,17 +10022,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="102" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C12" s="103">
         <v>9</v>
       </c>
       <c r="D12" s="102" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E12" s="104"/>
       <c r="F12" s="105" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G12" s="106"/>
       <c r="H12" s="107"/>
@@ -10046,10 +10046,10 @@
       </c>
       <c r="M12" s="102"/>
       <c r="N12" s="102" t="s">
+        <v>354</v>
+      </c>
+      <c r="O12" s="102" t="s">
         <v>355</v>
-      </c>
-      <c r="O12" s="102" t="s">
-        <v>356</v>
       </c>
       <c r="P12" s="102"/>
       <c r="Q12" s="102"/>
@@ -10057,7 +10057,7 @@
       <c r="S12" s="102"/>
       <c r="T12" s="102"/>
       <c r="U12" s="108" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -10065,17 +10065,17 @@
         <v>11</v>
       </c>
       <c r="B13" s="102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C13" s="103">
         <v>10</v>
       </c>
       <c r="D13" s="102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E13" s="104"/>
       <c r="F13" s="105" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G13" s="106"/>
       <c r="H13" s="107"/>
@@ -10089,10 +10089,10 @@
       </c>
       <c r="M13" s="102"/>
       <c r="N13" s="102" t="s">
+        <v>358</v>
+      </c>
+      <c r="O13" s="102" t="s">
         <v>359</v>
-      </c>
-      <c r="O13" s="102" t="s">
-        <v>360</v>
       </c>
       <c r="P13" s="102"/>
       <c r="Q13" s="102"/>
@@ -10100,7 +10100,7 @@
       <c r="S13" s="102"/>
       <c r="T13" s="102"/>
       <c r="U13" s="108" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -10108,17 +10108,17 @@
         <v>12</v>
       </c>
       <c r="B14" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C14" s="103">
         <v>11</v>
       </c>
       <c r="D14" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E14" s="104"/>
       <c r="F14" s="105" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G14" s="106"/>
       <c r="H14" s="107"/>
@@ -10132,18 +10132,18 @@
       </c>
       <c r="M14" s="102"/>
       <c r="N14" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="O14" s="102"/>
       <c r="P14" s="102" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="Q14" s="102"/>
       <c r="R14" s="102"/>
       <c r="S14" s="102"/>
       <c r="T14" s="102"/>
       <c r="U14" s="108" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -10151,17 +10151,17 @@
         <v>13</v>
       </c>
       <c r="B15" s="102" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C15" s="103">
         <v>12</v>
       </c>
       <c r="D15" s="102" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E15" s="104"/>
       <c r="F15" s="105" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G15" s="106"/>
       <c r="H15" s="107"/>
@@ -10175,24 +10175,24 @@
       </c>
       <c r="M15" s="102"/>
       <c r="N15" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O15" s="102"/>
       <c r="P15" s="102" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q15" s="102" t="s">
         <v>368</v>
       </c>
-      <c r="Q15" s="102" t="s">
+      <c r="R15" s="102" t="s">
         <v>369</v>
-      </c>
-      <c r="R15" s="102" t="s">
-        <v>370</v>
       </c>
       <c r="S15" s="102"/>
       <c r="T15" s="102" t="s">
+        <v>370</v>
+      </c>
+      <c r="U15" s="108" t="s">
         <v>371</v>
-      </c>
-      <c r="U15" s="108" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -10200,24 +10200,24 @@
         <v>14</v>
       </c>
       <c r="B16" s="102" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C16" s="103">
         <v>13</v>
       </c>
       <c r="D16" s="102" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E16" s="104"/>
       <c r="F16" s="105" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G16" s="106"/>
       <c r="H16" s="107" t="s">
+        <v>373</v>
+      </c>
+      <c r="I16" s="107" t="s">
         <v>374</v>
-      </c>
-      <c r="I16" s="107" t="s">
-        <v>375</v>
       </c>
       <c r="J16" s="106"/>
       <c r="K16" s="102">
@@ -10228,24 +10228,24 @@
       </c>
       <c r="M16" s="102"/>
       <c r="N16" s="102" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O16" s="102"/>
       <c r="P16" s="102" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q16" s="102" t="s">
         <v>377</v>
       </c>
-      <c r="Q16" s="102" t="s">
+      <c r="R16" s="102" t="s">
         <v>378</v>
-      </c>
-      <c r="R16" s="102" t="s">
-        <v>379</v>
       </c>
       <c r="S16" s="102"/>
       <c r="T16" s="102" t="s">
+        <v>379</v>
+      </c>
+      <c r="U16" s="108" t="s">
         <v>380</v>
-      </c>
-      <c r="U16" s="108" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -10253,13 +10253,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C17" s="89">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E17" s="90"/>
       <c r="F17" s="91"/>
@@ -10270,17 +10270,17 @@
         <v>16</v>
       </c>
       <c r="B18" s="102" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C18" s="103">
         <v>15</v>
       </c>
       <c r="D18" s="102" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E18" s="104"/>
       <c r="F18" s="105" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G18" s="106"/>
       <c r="H18" s="107"/>
@@ -10294,24 +10294,24 @@
       </c>
       <c r="M18" s="102"/>
       <c r="N18" s="102" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O18" s="102"/>
       <c r="P18" s="102" t="s">
+        <v>383</v>
+      </c>
+      <c r="Q18" s="102" t="s">
         <v>384</v>
       </c>
-      <c r="Q18" s="102" t="s">
+      <c r="R18" s="102" t="s">
         <v>385</v>
-      </c>
-      <c r="R18" s="102" t="s">
-        <v>386</v>
       </c>
       <c r="S18" s="102"/>
       <c r="T18" s="102" t="s">
+        <v>386</v>
+      </c>
+      <c r="U18" s="108" t="s">
         <v>387</v>
-      </c>
-      <c r="U18" s="108" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -10319,18 +10319,18 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C19" s="89">
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E19" s="90"/>
       <c r="F19" s="91"/>
       <c r="G19" s="93" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H19" s="94"/>
       <c r="I19" s="94"/>
@@ -10339,10 +10339,10 @@
         <v>9</v>
       </c>
       <c r="R19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S19" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="U19" s="92"/>
     </row>
@@ -10351,18 +10351,18 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C20" s="89">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E20" s="90"/>
       <c r="F20" s="91"/>
       <c r="G20" s="93" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H20" s="94"/>
       <c r="I20" s="94"/>
@@ -10371,10 +10371,10 @@
         <v>10</v>
       </c>
       <c r="R20" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="S20" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="U20" s="92"/>
     </row>
@@ -10394,7 +10394,7 @@
       <c r="E21" s="90"/>
       <c r="F21" s="91"/>
       <c r="G21" s="93" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H21" s="94"/>
       <c r="I21" s="94"/>
@@ -10403,7 +10403,7 @@
         <v>11</v>
       </c>
       <c r="R21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="S21" t="s">
         <v>176</v>
@@ -10415,7 +10415,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E22" s="90"/>
       <c r="F22" s="91"/>
@@ -10430,13 +10430,13 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C23" s="89">
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E23" s="90"/>
       <c r="F23" s="91"/>
@@ -10450,10 +10450,10 @@
         <v>6</v>
       </c>
       <c r="R23" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="U23" s="92"/>
     </row>
@@ -10462,13 +10462,13 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C24" s="89">
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E24" s="90"/>
       <c r="F24" s="91"/>
@@ -10482,10 +10482,10 @@
         <v>7</v>
       </c>
       <c r="R24" t="s">
+        <v>399</v>
+      </c>
+      <c r="S24" t="s">
         <v>400</v>
-      </c>
-      <c r="S24" t="s">
-        <v>401</v>
       </c>
       <c r="U24" s="92"/>
     </row>
@@ -10494,13 +10494,13 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C25" s="89">
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E25" s="90"/>
       <c r="F25" s="91"/>
@@ -10514,10 +10514,10 @@
         <v>8</v>
       </c>
       <c r="R25" t="s">
+        <v>402</v>
+      </c>
+      <c r="S25" t="s">
         <v>403</v>
-      </c>
-      <c r="S25" t="s">
-        <v>404</v>
       </c>
       <c r="U25" s="92"/>
     </row>
@@ -10526,24 +10526,24 @@
         <v>23</v>
       </c>
       <c r="B26" s="102" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C26" s="103">
         <v>23</v>
       </c>
       <c r="D26" s="102" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E26" s="107"/>
       <c r="F26" s="105" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G26" s="106"/>
       <c r="H26" s="107" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I26" s="107" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J26" s="106"/>
       <c r="K26" s="102">
@@ -10554,24 +10554,24 @@
       </c>
       <c r="M26" s="102"/>
       <c r="N26" s="102" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="O26" s="102"/>
       <c r="P26" s="102" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q26" s="102" t="s">
         <v>408</v>
       </c>
-      <c r="Q26" s="102" t="s">
+      <c r="R26" s="102" t="s">
         <v>409</v>
-      </c>
-      <c r="R26" s="102" t="s">
-        <v>410</v>
       </c>
       <c r="S26" s="102"/>
       <c r="T26" s="102" t="s">
         <v>176</v>
       </c>
       <c r="U26" s="108" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -10579,26 +10579,26 @@
         <v>24</v>
       </c>
       <c r="B27" s="102" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C27" s="103">
         <v>24</v>
       </c>
       <c r="D27" s="102" t="s">
+        <v>411</v>
+      </c>
+      <c r="E27" s="104" t="s">
         <v>412</v>
       </c>
-      <c r="E27" s="104" t="s">
-        <v>413</v>
-      </c>
       <c r="F27" s="105" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G27" s="106"/>
       <c r="H27" s="107" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I27" s="107" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J27" s="106"/>
       <c r="K27" s="102">
@@ -10609,19 +10609,19 @@
       </c>
       <c r="M27" s="102"/>
       <c r="N27" s="102" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="O27" s="102"/>
       <c r="P27" s="102" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q27" s="102"/>
       <c r="R27" s="102" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="S27" s="102"/>
       <c r="T27" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="U27" s="108"/>
     </row>
@@ -10630,26 +10630,26 @@
         <v>25</v>
       </c>
       <c r="B28" s="102" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C28" s="103">
         <v>25</v>
       </c>
       <c r="D28" s="102" t="s">
+        <v>417</v>
+      </c>
+      <c r="E28" s="104" t="s">
         <v>418</v>
       </c>
-      <c r="E28" s="104" t="s">
-        <v>419</v>
-      </c>
       <c r="F28" s="105" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G28" s="106"/>
       <c r="H28" s="107" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I28" s="107" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J28" s="106"/>
       <c r="K28" s="102">
@@ -10660,20 +10660,20 @@
       </c>
       <c r="M28" s="102"/>
       <c r="N28" s="102" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="O28" s="102"/>
       <c r="P28" s="102" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="Q28" s="102"/>
       <c r="R28" s="102"/>
       <c r="S28" s="102"/>
       <c r="T28" s="102" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="U28" s="108" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -10681,17 +10681,17 @@
         <v>26</v>
       </c>
       <c r="B29" s="102" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C29" s="103">
         <v>26</v>
       </c>
       <c r="D29" s="102" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E29" s="104"/>
       <c r="F29" s="105" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G29" s="106"/>
       <c r="H29" s="107"/>
@@ -10705,20 +10705,20 @@
       </c>
       <c r="M29" s="102"/>
       <c r="N29" s="102" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O29" s="102"/>
       <c r="P29" s="102" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Q29" s="102"/>
       <c r="R29" s="102" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="S29" s="102"/>
       <c r="T29" s="102"/>
       <c r="U29" s="108" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -10726,17 +10726,17 @@
         <v>27</v>
       </c>
       <c r="B30" s="102" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C30" s="103">
         <v>27</v>
       </c>
       <c r="D30" s="102" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E30" s="104"/>
       <c r="F30" s="105" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G30" s="106"/>
       <c r="H30" s="107"/>
@@ -10755,7 +10755,7 @@
       <c r="S30" s="102"/>
       <c r="T30" s="102"/>
       <c r="U30" s="108" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -10763,17 +10763,17 @@
         <v>28</v>
       </c>
       <c r="B31" s="102" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C31" s="103">
         <v>28</v>
       </c>
       <c r="D31" s="102" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E31" s="104"/>
       <c r="F31" s="105" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G31" s="106"/>
       <c r="H31" s="107"/>
@@ -10792,7 +10792,7 @@
       <c r="S31" s="102"/>
       <c r="T31" s="102"/>
       <c r="U31" s="108" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -10800,24 +10800,24 @@
         <v>29</v>
       </c>
       <c r="B32" s="102" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C32" s="103">
         <v>29</v>
       </c>
       <c r="D32" s="102" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E32" s="104"/>
       <c r="F32" s="105" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G32" s="106"/>
       <c r="H32" s="107" t="s">
         <v>130</v>
       </c>
       <c r="I32" s="107" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J32" s="106"/>
       <c r="K32" s="102"/>
@@ -10830,12 +10830,12 @@
       <c r="P32" s="102"/>
       <c r="Q32" s="102"/>
       <c r="R32" s="102" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="S32" s="102"/>
       <c r="T32" s="102"/>
       <c r="U32" s="108" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -10843,17 +10843,17 @@
         <v>30</v>
       </c>
       <c r="B33" s="102" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C33" s="103">
         <v>30</v>
       </c>
       <c r="D33" s="102" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E33" s="104"/>
       <c r="F33" s="105" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G33" s="106"/>
       <c r="H33" s="107"/>
@@ -10869,7 +10869,7 @@
       <c r="P33" s="102"/>
       <c r="Q33" s="102"/>
       <c r="R33" s="102" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="S33" s="102"/>
       <c r="T33" s="102"/>
@@ -10880,17 +10880,17 @@
         <v>31</v>
       </c>
       <c r="B34" s="102" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C34" s="103">
         <v>31</v>
       </c>
       <c r="D34" s="102" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E34" s="104"/>
       <c r="F34" s="105" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G34" s="106"/>
       <c r="H34" s="107"/>
@@ -10906,12 +10906,12 @@
       <c r="P34" s="102"/>
       <c r="Q34" s="102"/>
       <c r="R34" s="102" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="S34" s="102"/>
       <c r="T34" s="102"/>
       <c r="U34" s="108" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -10936,17 +10936,17 @@
         <v>33</v>
       </c>
       <c r="B36" s="102" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C36" s="103">
         <v>33</v>
       </c>
       <c r="D36" s="102" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E36" s="104"/>
       <c r="F36" s="105" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G36" s="106"/>
       <c r="H36" s="107"/>
@@ -10962,12 +10962,12 @@
       <c r="P36" s="102"/>
       <c r="Q36" s="102"/>
       <c r="R36" s="102" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="S36" s="102"/>
       <c r="T36" s="102"/>
       <c r="U36" s="108" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -10975,17 +10975,17 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C37" s="89">
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E37" s="90"/>
       <c r="F37" s="91" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G37" s="93"/>
       <c r="H37" s="94"/>
@@ -11001,17 +11001,17 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C38" s="89">
         <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E38" s="90"/>
       <c r="F38" s="91" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G38" s="93"/>
       <c r="H38" s="94"/>
@@ -11021,7 +11021,7 @@
         <v>1</v>
       </c>
       <c r="U38" s="92" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -11029,17 +11029,17 @@
         <v>36</v>
       </c>
       <c r="B39" s="102" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C39" s="103">
         <v>36</v>
       </c>
       <c r="D39" s="102" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E39" s="104"/>
       <c r="F39" s="105" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G39" s="106"/>
       <c r="H39" s="107"/>
@@ -11055,12 +11055,12 @@
       <c r="P39" s="102"/>
       <c r="Q39" s="102"/>
       <c r="R39" s="102" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="S39" s="102"/>
       <c r="T39" s="102"/>
       <c r="U39" s="108" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -11068,17 +11068,17 @@
         <v>37</v>
       </c>
       <c r="B40" s="102" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C40" s="103">
         <v>37</v>
       </c>
       <c r="D40" s="102" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E40" s="104"/>
       <c r="F40" s="105" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G40" s="106"/>
       <c r="H40" s="107"/>
@@ -11094,7 +11094,7 @@
       <c r="P40" s="102"/>
       <c r="Q40" s="102"/>
       <c r="R40" s="102" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="S40" s="102"/>
       <c r="T40" s="102"/>
@@ -11105,13 +11105,13 @@
         <v>38</v>
       </c>
       <c r="B41" s="109" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C41" s="110">
         <v>38</v>
       </c>
       <c r="D41" s="109" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E41" s="111"/>
       <c r="F41" s="112"/>
@@ -11134,18 +11134,18 @@
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="102"/>
       <c r="B43" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="95"/>
       <c r="B44" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>